<commit_message>
1. Added Test case for app repository. 2. added new test data excel sheet
</commit_message>
<xml_diff>
--- a/MDM/TestData/Excel/New_MDMTestData.xlsx
+++ b/MDM/TestData/Excel/New_MDMTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14550" windowHeight="2865" tabRatio="909" activeTab="11"/>
+    <workbookView windowWidth="19890" windowHeight="8355" tabRatio="909" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="APKs" sheetId="11" r:id="rId10"/>
     <sheet name="DBQueries" sheetId="12" r:id="rId11"/>
     <sheet name="Devices" sheetId="13" r:id="rId12"/>
+    <sheet name="Nw Config" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:B6"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197">
   <si>
     <t>Userrole</t>
   </si>
@@ -584,9 +585,6 @@
     <t xml:space="preserve">SIMID </t>
   </si>
   <si>
-    <t>8991272172933070000</t>
-  </si>
-  <si>
     <t>UpdatedDeviceName</t>
   </si>
   <si>
@@ -600,6 +598,27 @@
   </si>
   <si>
     <t>UpdatedGroup</t>
+  </si>
+  <si>
+    <t>AppInventorySearch</t>
+  </si>
+  <si>
+    <t>ES File Explorer</t>
+  </si>
+  <si>
+    <t>Network Usage Configuration</t>
+  </si>
+  <si>
+    <t>AutomationNetwo...</t>
+  </si>
+  <si>
+    <t>Billing Cycle Start Date</t>
+  </si>
+  <si>
+    <t>Mobile Data Plan Limit</t>
+  </si>
+  <si>
+    <t>500 MB</t>
   </si>
 </sst>
 </file>
@@ -609,10 +628,10 @@
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="0_);\(0\)"/>
+    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="179" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="180" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="181" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="181" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -623,9 +642,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
       <charset val="134"/>
     </font>
     <font>
@@ -660,110 +679,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -779,6 +700,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -786,6 +745,66 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="38">
     <fill>
@@ -826,187 +845,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1057,11 +1076,46 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1082,30 +1136,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1120,28 +1150,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1150,7 +1169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1162,167 +1181,161 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1386,13 +1399,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="5" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="5" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1405,12 +1418,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="10" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1769,50 +1776,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="34" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="34" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="34" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1845,194 +1852,194 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="11">
+      <c r="A2" s="9">
         <v>2048</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="6" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="6" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="6" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="6" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="6" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="6" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="6" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="6" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="6" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="6" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="6" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="6" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="6" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2058,18 +2065,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2077,15 +2084,15 @@
       <c r="A3" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2130,23 +2137,23 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="34.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2166,7 +2173,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" ht="21" customHeight="1" spans="1:2">
+    <row r="4" ht="31.5" spans="1:2">
       <c r="A4" t="s">
         <v>172</v>
       </c>
@@ -2183,10 +2190,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>176</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2194,7 +2201,7 @@
       <c r="A7" t="s">
         <v>178</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2202,7 +2209,7 @@
       <c r="A8" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2210,7 +2217,7 @@
       <c r="A9" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2218,32 +2225,104 @@
       <c r="A10" t="s">
         <v>184</v>
       </c>
-      <c r="B10" s="38" t="s">
-        <v>185</v>
+      <c r="B10">
+        <v>8.99127217293307e+18</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11" t="s">
         <v>186</v>
-      </c>
-      <c r="B11" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" t="s">
         <v>188</v>
-      </c>
-      <c r="B12" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -2268,26 +2347,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2309,7 +2388,7 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="13.25" customWidth="1"/>
-    <col min="2" max="2" width="24.25" style="30" customWidth="1"/>
+    <col min="2" max="2" width="24.25" style="28" customWidth="1"/>
     <col min="3" max="3" width="16.25" customWidth="1"/>
     <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
@@ -2317,50 +2396,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="29" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="29" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2368,7 +2447,7 @@
       <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="31" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2397,18 +2476,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2434,18 +2513,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2471,18 +2550,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2497,152 +2576,152 @@
   <sheetPr/>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="29.125" customWidth="1"/>
-    <col min="2" max="2" width="38.125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="38.125" style="18" customWidth="1"/>
     <col min="3" max="3" width="15.25" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="22.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="21">
         <v>123456</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>9876543210</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="19" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="9">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="9">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="19" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="9">
         <v>7828342623</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="19" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="26" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="27" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2671,7 +2750,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>69</v>
       </c>
       <c r="B1" t="s">
@@ -2682,7 +2761,7 @@
       <c r="A2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2690,7 +2769,7 @@
       <c r="A3" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2698,27 +2777,27 @@
       <c r="A4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="18"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
@@ -2768,100 +2847,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="14"/>
+      <c r="B3" s="12"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="B9" s="14"/>
+      <c r="B9" s="12"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="10" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Test cases of Groups, UserRoles from Lavina Machine Added 2 test cases of Devices from lavina machine Added updated New Mdm Test data excel sheet Updated the OR
</commit_message>
<xml_diff>
--- a/MDM/TestData/Excel/New_MDMTestData.xlsx
+++ b/MDM/TestData/Excel/New_MDMTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="8355" tabRatio="909" activeTab="11"/>
+    <workbookView windowWidth="20385" windowHeight="8340" tabRatio="909" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Fences" sheetId="10" r:id="rId9"/>
     <sheet name="APKs" sheetId="11" r:id="rId10"/>
     <sheet name="DBQueries" sheetId="12" r:id="rId11"/>
-    <sheet name="Devices" sheetId="13" r:id="rId12"/>
-    <sheet name="Nw Config" sheetId="14" r:id="rId13"/>
+    <sheet name="Nw Config" sheetId="14" r:id="rId12"/>
+    <sheet name="Devices" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:B6"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213">
   <si>
     <t>Userrole</t>
   </si>
@@ -131,13 +131,61 @@
     <t>This is automation group.</t>
   </si>
   <si>
-    <t>User Role Name</t>
+    <t>UpdatedGroupName</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>NewGroupName</t>
+  </si>
+  <si>
+    <t>Dummy Automation Group</t>
+  </si>
+  <si>
+    <t>UpdatedPolicy</t>
+  </si>
+  <si>
+    <t>Policy ALL</t>
+  </si>
+  <si>
+    <t>UpdatedFenceConfiguration</t>
+  </si>
+  <si>
+    <t>Automation_Fence</t>
+  </si>
+  <si>
+    <t>GroupAddDevice</t>
+  </si>
+  <si>
+    <t>Nexus Test</t>
+  </si>
+  <si>
+    <t>GroupAssignOwner</t>
+  </si>
+  <si>
+    <t>Automation User</t>
+  </si>
+  <si>
+    <t>UserRoleName</t>
   </si>
   <si>
     <t>SemiAdvance</t>
   </si>
   <si>
-    <t>User Role Type</t>
+    <t>UserRoleType</t>
+  </si>
+  <si>
+    <t>UpdatedUserRoleType</t>
+  </si>
+  <si>
+    <t>NewUserRoleName</t>
+  </si>
+  <si>
+    <t>NewUserRoleType</t>
+  </si>
+  <si>
+    <t>Advanced</t>
   </si>
   <si>
     <t>PolicyName</t>
@@ -530,10 +578,31 @@
     <t>Select count(*) from device where is_locked=1</t>
   </si>
   <si>
+    <t>Network Usage Configuration</t>
+  </si>
+  <si>
+    <t>AutomationNetwo...</t>
+  </si>
+  <si>
+    <t>Billing Cycle Start Date</t>
+  </si>
+  <si>
+    <t>07-08-2018</t>
+  </si>
+  <si>
+    <t>Mobile Data Plan Limit</t>
+  </si>
+  <si>
+    <t>500 MB</t>
+  </si>
+  <si>
     <t>DeviceName</t>
   </si>
   <si>
     <t>Demo Non-KNOX One Plus Three</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
   <si>
     <t>Owner</t>
@@ -588,15 +657,9 @@
     <t>UpdatedDeviceName</t>
   </si>
   <si>
-    <t>xyz</t>
-  </si>
-  <si>
     <t>UpdatedOwner</t>
   </si>
   <si>
-    <t>Automation User</t>
-  </si>
-  <si>
     <t>UpdatedGroup</t>
   </si>
   <si>
@@ -604,34 +667,18 @@
   </si>
   <si>
     <t>ES File Explorer</t>
-  </si>
-  <si>
-    <t>Network Usage Configuration</t>
-  </si>
-  <si>
-    <t>AutomationNetwo...</t>
-  </si>
-  <si>
-    <t>Billing Cycle Start Date</t>
-  </si>
-  <si>
-    <t>Mobile Data Plan Limit</t>
-  </si>
-  <si>
-    <t>500 MB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="179" formatCode="dd/mm/yyyy"/>
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="180" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="181" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -640,12 +687,6 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -670,61 +711,15 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -739,7 +734,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -754,8 +749,75 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -770,30 +832,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -805,6 +845,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="38">
     <fill>
@@ -845,31 +892,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -881,13 +1018,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -899,133 +1030,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1070,8 +1117,73 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1095,72 +1207,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1169,148 +1216,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1318,19 +1365,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -1339,7 +1383,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1348,7 +1392,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
@@ -1360,7 +1404,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1396,16 +1440,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="5" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1417,7 +1464,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="10" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="10" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1784,7 +1831,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="34" t="s">
@@ -1792,7 +1839,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="34" t="s">
@@ -1800,7 +1847,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="34" t="s">
@@ -1808,7 +1855,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="34" t="s">
@@ -1816,7 +1863,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="34" t="s">
@@ -1852,195 +1899,195 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>105</v>
+      <c r="A1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>2048</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>106</v>
+      <c r="B2" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>108</v>
+      <c r="A3" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>110</v>
+      <c r="A4" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>112</v>
+      <c r="A5" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>114</v>
+      <c r="A6" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>116</v>
+      <c r="A7" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>118</v>
+      <c r="A8" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>120</v>
+      <c r="A9" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>122</v>
+      <c r="A10" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>124</v>
+      <c r="A11" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>126</v>
+      <c r="A12" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>128</v>
+      <c r="A13" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>130</v>
+      <c r="A14" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>132</v>
+      <c r="A15" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>134</v>
+      <c r="A16" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>136</v>
+      <c r="A17" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>138</v>
+      <c r="A18" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>140</v>
+      <c r="A19" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>142</v>
+      <c r="A20" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>144</v>
+      <c r="A21" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>146</v>
+      <c r="A22" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>148</v>
+      <c r="A23" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>150</v>
+      <c r="A24" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2065,67 +2112,67 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:2">
-      <c r="A1" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>152</v>
+      <c r="A1" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:2">
-      <c r="A2" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>154</v>
+      <c r="A2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:2">
       <c r="A3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>156</v>
+        <v>171</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:2">
-      <c r="A4" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>158</v>
+      <c r="A4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:2">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:2">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="1:2">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:2">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="B8" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2137,132 +2184,57 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="34.875" customWidth="1"/>
+    <col min="2" max="2" width="30" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>183</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B2" t="s">
-        <v>170</v>
+        <v>185</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" ht="31.5" spans="1:2">
+        <v>187</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>180</v>
-      </c>
-      <c r="B8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B9" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>184</v>
-      </c>
-      <c r="B10">
-        <v>8.99127217293307e+18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>185</v>
-      </c>
-      <c r="B11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>187</v>
-      </c>
-      <c r="B12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>189</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>190</v>
-      </c>
-      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -2273,56 +2245,128 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="34.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
+      </c>
+      <c r="B1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B2" s="2">
-        <v>43319</v>
+        <v>192</v>
+      </c>
+      <c r="B2" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" ht="31.5" spans="1:2">
+      <c r="A4" t="s">
         <v>195</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5">
-        <v>321</v>
+        <v>197</v>
+      </c>
+      <c r="B5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" s="2">
+        <v>8.99127e+18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>210</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2355,18 +2399,18 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2381,8 +2425,8 @@
   <sheetPr/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="1"/>
@@ -2396,7 +2440,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="29" t="s">
@@ -2404,7 +2448,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="29" t="s">
@@ -2412,7 +2456,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="30" t="s">
@@ -2420,23 +2464,23 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="29" t="s">
@@ -2463,32 +2507,80 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="7" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="25.625" customWidth="1"/>
     <col min="2" max="2" width="34.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2500,32 +2592,56 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="17.125" customWidth="1"/>
+    <col min="1" max="1" width="19.875" customWidth="1"/>
     <col min="2" max="2" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>4</v>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2550,19 +2666,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>38</v>
+      <c r="A1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>40</v>
+      <c r="A2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2583,146 +2699,146 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="29.125" customWidth="1"/>
-    <col min="2" max="2" width="38.125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="38.125" style="17" customWidth="1"/>
     <col min="3" max="3" width="15.25" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="22.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>42</v>
+      <c r="A1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>44</v>
+      <c r="A2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="21">
+      <c r="A3" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="20">
         <v>123456</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>47</v>
+      <c r="A4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="9">
+      <c r="A5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="8">
         <v>9876543210</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="9">
-        <v>50</v>
-      </c>
-    </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="9">
+      <c r="A10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="8">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>57</v>
+      <c r="A11" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="9">
+      <c r="A12" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="8">
         <v>7828342623</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>60</v>
+      <c r="A13" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>62</v>
+      <c r="A14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>64</v>
+      <c r="A15" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>66</v>
+      <c r="A16" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>68</v>
+      <c r="A17" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2750,73 +2866,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="8" t="s">
-        <v>69</v>
+      <c r="A1" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>72</v>
+        <v>87</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>74</v>
+        <v>89</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>76</v>
+        <v>91</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="A6" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="16"/>
+      <c r="A7" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2847,101 +2963,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>84</v>
+      <c r="A1" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>86</v>
+      <c r="A2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="12"/>
+      <c r="A3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>89</v>
+      <c r="A4" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>91</v>
+      <c r="A5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>93</v>
+      <c r="A6" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="12"/>
+      <c r="A7" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="11"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>96</v>
+      <c r="A8" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="12"/>
+      <c r="A9" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="11"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>99</v>
+      <c r="A10" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>100</v>
+      <c r="B11" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>102</v>
+      <c r="A12" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>104</v>
+      <c r="A13" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>